<commit_message>
Correct an error in the breakdown comment make the breakdown error grammar make sense add in lsips into fe resources
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{DF84BD86-762B-4D46-B16D-17AC86338A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017BFB79-D56F-49CB-BB43-F76775AA17B7}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{DF84BD86-762B-4D46-B16D-17AC86338A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{962A0115-AB18-46A2-BB2A-A4979A5D3A71}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -286,9 +286,6 @@
     <t>Employment in</t>
   </si>
   <si>
-    <t>employment volume</t>
-  </si>
-  <si>
     <t>Employment is</t>
   </si>
   <si>
@@ -334,9 +331,6 @@
     <t>Online job adverts</t>
   </si>
   <si>
-    <t>number of online job adverts</t>
-  </si>
-  <si>
     <t>The number of online job adverts is</t>
   </si>
   <si>
@@ -349,9 +343,6 @@
     <t>Businesses</t>
   </si>
   <si>
-    <t>number of businesses</t>
-  </si>
-  <si>
     <t>The number of businesses is</t>
   </si>
   <si>
@@ -391,9 +382,6 @@
     <t>FE achievements</t>
   </si>
   <si>
-    <t>number of FE achievements</t>
-  </si>
-  <si>
     <t>FE achievements are</t>
   </si>
   <si>
@@ -401,9 +389,6 @@
   </si>
   <si>
     <t>FE participation</t>
-  </si>
-  <si>
-    <t>FE participation volume</t>
   </si>
   <si>
     <t>FE participation is</t>
@@ -691,6 +676,21 @@
   </si>
   <si>
     <t>Apr 2022 - Mar 2023 data</t>
+  </si>
+  <si>
+    <t>share of businesses</t>
+  </si>
+  <si>
+    <t>FE participation share</t>
+  </si>
+  <si>
+    <t>share of FE achievements</t>
+  </si>
+  <si>
+    <t>share of online job adverts</t>
+  </si>
+  <si>
+    <t>employment volume share</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1145,30 +1145,30 @@
         <v>58</v>
       </c>
       <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" t="s">
         <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -1180,13 +1180,13 @@
         <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>60</v>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>27</v>
@@ -1221,13 +1221,13 @@
         <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>41</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>65</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>27</v>
@@ -1262,13 +1262,13 @@
         <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>60</v>
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>27</v>
@@ -1303,13 +1303,13 @@
         <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>72</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="6" spans="1:13" ht="261.5" thickBot="1">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -1344,13 +1344,13 @@
         <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>76</v>
@@ -1362,18 +1362,18 @@
         <v>75</v>
       </c>
       <c r="L6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>27</v>
@@ -1385,36 +1385,36 @@
         <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>27</v>
@@ -1426,36 +1426,36 @@
         <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>27</v>
@@ -1467,28 +1467,28 @@
         <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>46</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L9" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="203.5" thickBot="1">
@@ -1496,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
@@ -1508,28 +1508,28 @@
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>47</v>
       </c>
       <c r="J10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="M10" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="145.5" thickBot="1">
@@ -1537,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>28</v>
@@ -1549,28 +1549,28 @@
         <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I11" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="319.5" thickBot="1">
@@ -1578,7 +1578,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>28</v>
@@ -1590,28 +1590,28 @@
         <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>49</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="319.5" thickBot="1">
@@ -1619,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>28</v>
@@ -1631,28 +1631,28 @@
         <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>50</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
@@ -1660,7 +1660,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>32</v>
@@ -1672,28 +1672,28 @@
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>51</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>112</v>
+        <v>193</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1701,7 +1701,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>33</v>
@@ -1713,28 +1713,28 @@
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>52</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1742,7 +1742,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>38</v>
@@ -1754,28 +1754,28 @@
         <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1783,7 +1783,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>39</v>
@@ -1795,39 +1795,39 @@
         <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
@@ -1836,28 +1836,28 @@
         <v>27</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>55</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>55</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
@@ -1865,7 +1865,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1877,28 +1877,28 @@
         <v>35</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>56</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="254" thickBot="1">
@@ -1906,7 +1906,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
         <v>36</v>
@@ -1918,66 +1918,66 @@
         <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>57</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>57</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="409.6" thickBot="1">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E21" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>76</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="M21" s="8"/>
     </row>
@@ -1986,7 +1986,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>31</v>
@@ -1998,7 +1998,7 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2007,7 +2007,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>33</v>
@@ -2019,7 +2019,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
change ks4 caveat to be clearer
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-2_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1621E2-8717-428A-B1C0-0FDBED89DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8807B596-198D-4A57-8AB5-676F372A681D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -687,17 +687,17 @@
     <t>Mar 2023 data</t>
   </si>
   <si>
+    <t>Jul 2022 - Jun 2023 data</t>
+  </si>
+  <si>
     <t>&lt;ol&gt;
-&lt;li&gt;The way it is decided when a student is at the end of 16 to 18 study has changed this year and comparisons to previous cohorts should be treated with caution. Students are included in this statistical release when they reach the end of 16 to 18 study. The ‘trigger’ rules for deciding when this happens changed in 2020/21. Further details can be found in the &lt;a href = https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures'&gt;publication&lt;/a&gt;.&lt;/li&gt;
+&lt;li&gt;The definition of when a student is at the end of 16 to 18 study has changed this year and comparisons to previous cohorts should be treated with caution. Students are included in this statistical release when they reach the end of 16 to 18 study. The ‘trigger’ rules for deciding when this happens changed in 2020/21. Further details can be found in the &lt;a href = https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures'&gt;publication&lt;/a&gt;.&lt;/li&gt;
 &lt;li&gt;There was no checking exercise for this cohort of students. The checking exercise ordinarily allows schools and colleges to confirm whether the students we report are at end of 16 to 18 study. This means that this data may not accurately represent whether students were at the end of 16 to 18 study in 2020/21.&lt;/li&gt;
   &lt;li&gt;Data based on destinations of state-funded mainstream schools and colleges.&lt;/li&gt;
  &lt;li&gt;There is no double counting across destinations, a young person is reported in one destination category only.&lt;/li&gt;
  &lt;li&gt;If a student is registered as being in education and an apprenticeship, it is recorded as a sustained education and if a student is registered in employment along with an apprenticeship or in education, it is recorded as sustained employment.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>Jul 2022 - Jun 2023 data</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1175,7 +1175,7 @@
         <v>167</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>25</v>
@@ -1216,7 +1216,7 @@
         <v>169</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>25</v>
@@ -1257,7 +1257,7 @@
         <v>170</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>25</v>
@@ -1298,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>25</v>
@@ -1339,7 +1339,7 @@
         <v>168</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>25</v>
@@ -1380,7 +1380,7 @@
         <v>171</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>25</v>
@@ -1421,7 +1421,7 @@
         <v>172</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>25</v>
@@ -1462,7 +1462,7 @@
         <v>173</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>25</v>
@@ -1925,7 +1925,7 @@
         <v>192</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
119	Employment volumes are for 16-64 year olds.  This should really be shown for 16+ to show all employment – that’s the figure ONS and nomis tend to lead on. This may be to allign with other metrics - need to check that before changing 213	Employment volumes.  For the occupation and industry figures by LADU they all look odd.  I think his is because there must be suppressed figures in the volumes, then the percentages are calculated from the sum of the un-suppressed figures?  Example below – it means you only get 4-5 occupations and they are so much higher than anything else.  If I’ve got the reason wrong, the figures still look dubious.  If there’s not an easy fix we should just remove the LADU figures entirely.
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A66D6684-2770-4125-B438-E3BE62AD7DF1}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5653A26-6F19-4C2D-9155-F86ECD6A1434}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -517,13 +517,6 @@
   </si>
   <si>
     <t>&lt;ol&gt;
-  &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
-&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
-&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
   &lt;li&gt;These statistics should be treated as experimental, as they are still subject to testing the ability to meet user needs.&lt;/li&gt;
 &lt;li&gt;Duplication of adverts can occur when the same job is posted on multiple job boards, or when multiple recruiters advertise the job at the same time.&lt;/li&gt;
 &lt;li&gt;Counts have been rounded to the nearest 5. Totals may not add due to this rounding.&lt;/li&gt;
@@ -625,16 +618,6 @@
     <t>Qualification estimates for the Jan 2022-Dec2022 survey period are temporarily suspended. The coding of qualifications has been changed to reflect an updated qualification framework. ONS have temporarily suspended the publication of these series while they update their datasets to reflect this change. They will reinstate qualification outputs as soon as they have made this update.</t>
   </si>
   <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Employment volumes are for 16-64 year olds.&lt;/li&gt;
-&lt;li&gt;Industry split volumes are for all ages. &lt;/li&gt;
-&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
-&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
-&lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
-&lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>share of businesses</t>
   </si>
   <si>
@@ -702,6 +685,22 @@
   <si>
     <t xml:space="preserve">	
 Oct 2022-Sep 2023</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Figures are for 16+ year olds.&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Employment volumes are for 16+ year olds.&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
+&lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
+&lt;/ol&gt;</t>
   </si>
 </sst>
 </file>
@@ -827,9 +826,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -867,7 +866,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -973,7 +972,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1115,7 +1114,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1125,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1179,10 +1178,10 @@
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
@@ -1194,7 +1193,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>33</v>
@@ -1220,10 +1219,10 @@
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>24</v>
@@ -1235,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>34</v>
@@ -1261,10 +1260,10 @@
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>24</v>
@@ -1276,7 +1275,7 @@
         <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>35</v>
@@ -1305,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -1317,7 +1316,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>36</v>
@@ -1341,12 +1340,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="261.5" thickBot="1">
+    <row r="6" spans="1:13" ht="247" thickBot="1">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>24</v>
@@ -1358,7 +1357,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
@@ -1376,7 +1375,7 @@
         <v>68</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>70</v>
@@ -1384,10 +1383,10 @@
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>24</v>
@@ -1399,7 +1398,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>37</v>
@@ -1425,10 +1424,10 @@
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>24</v>
@@ -1440,7 +1439,7 @@
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>38</v>
@@ -1466,10 +1465,10 @@
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>24</v>
@@ -1481,7 +1480,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>39</v>
@@ -1522,7 +1521,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>40</v>
@@ -1540,7 +1539,7 @@
         <v>83</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>85</v>
@@ -1551,7 +1550,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>25</v>
@@ -1563,7 +1562,7 @@
         <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>41</v>
@@ -1581,7 +1580,7 @@
         <v>86</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>89</v>
@@ -1592,7 +1591,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>25</v>
@@ -1604,7 +1603,7 @@
         <v>25</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>42</v>
@@ -1633,7 +1632,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>25</v>
@@ -1645,7 +1644,7 @@
         <v>25</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>43</v>
@@ -1674,19 +1673,19 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>44</v>
@@ -1704,7 +1703,7 @@
         <v>101</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>102</v>
@@ -1715,19 +1714,19 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>45</v>
@@ -1745,7 +1744,7 @@
         <v>103</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>105</v>
@@ -1756,19 +1755,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>46</v>
@@ -1797,19 +1796,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>47</v>
@@ -1835,13 +1834,13 @@
     </row>
     <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
@@ -1850,7 +1849,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>48</v>
@@ -1882,16 +1881,16 @@
         <v>132</v>
       </c>
       <c r="C19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>49</v>
@@ -1923,16 +1922,16 @@
         <v>132</v>
       </c>
       <c r="C20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>50</v>
@@ -1958,22 +1957,22 @@
     </row>
     <row r="21" spans="1:13" ht="409.6" thickBot="1">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>130</v>
       </c>
       <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>133</v>
@@ -2000,19 +1999,19 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2021,19 +2020,19 @@
         <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
revert to 16-64 for employment data
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5653A26-6F19-4C2D-9155-F86ECD6A1434}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{210FF409-9903-4ECC-806E-3FAE1260A488}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -688,14 +688,15 @@
   </si>
   <si>
     <t>&lt;ol&gt;
-  &lt;li&gt;Figures are for 16+ year olds.&lt;/li&gt;
+  &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
 &lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
   <si>
     <t>&lt;ol&gt;
-  &lt;li&gt;Employment volumes are for 16+ year olds.&lt;/li&gt;
+  &lt;li&gt;Employment volumes are for 16-64 year olds.&lt;/li&gt;
+&lt;li&gt;Industry and occupation split volumes are for all ages.&lt;/li&gt;
 &lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
@@ -1124,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1340,7 +1341,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="247" thickBot="1">
+    <row r="6" spans="1:13" ht="276" thickBot="1">
       <c r="A6" t="s">
         <v>165</v>
       </c>

</xml_diff>

<commit_message>
changes following jane's qa
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{210FF409-9903-4ECC-806E-3FAE1260A488}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03AA0741-B64A-4F4A-BBA0-5F03ED59DB39}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -99,13 +99,7 @@
 Achievements are the number of learners who successfully complete an individual aim in an academic year.</t>
   </si>
   <si>
-    <t>This data is experimental. ONS are continuing to develop these statistics and aim to move to SOC profession grouping and publish data regularly. The timescale for the next release has not yet been agreed.</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;Annual Population Survey&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbyprofessionandlocalauthorityuk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
   <si>
     <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Counts&lt;/a&gt;</t>
@@ -436,9 +430,6 @@
   </si>
   <si>
     <t>Growth from 2023 to 2035</t>
-  </si>
-  <si>
-    <t>Dec 2022 data</t>
   </si>
   <si>
     <t>AY21/22 data</t>
@@ -702,6 +693,15 @@
 &lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
 &lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
 &lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>May 2023 data</t>
+  </si>
+  <si>
+    <t>This data is experimental. ONS are continuing to develop these statistics and aim to publish data regularly. The timescale for the next release has not yet been agreed.</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1141,10 +1141,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -1156,148 +1156,148 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" t="s">
         <v>124</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>125</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>126</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>127</v>
-      </c>
-      <c r="L1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="189" thickBot="1">
@@ -1305,204 +1305,204 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="276" thickBot="1">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="203.5" thickBot="1">
@@ -1510,40 +1510,40 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>195</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>195</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="M10" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="145.5" thickBot="1">
@@ -1551,40 +1551,40 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="319.5" thickBot="1">
@@ -1592,40 +1592,40 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="M12" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="319.5" thickBot="1">
@@ -1633,40 +1633,40 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="M13" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
@@ -1674,40 +1674,40 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I14" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1715,40 +1715,40 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="M15" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1756,40 +1756,40 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="M16" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1797,81 +1797,81 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="348.5" thickBot="1">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="263" thickBot="1">
@@ -1879,40 +1879,40 @@
         <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="L19" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="409.6" thickBot="1">
@@ -1920,78 +1920,78 @@
         <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="G20" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J20" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="M20" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="409.6" thickBot="1">
       <c r="A21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="F21" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C21" t="s">
-        <v>173</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E21" t="s">
-        <v>174</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G21" s="8" t="s">
+      <c r="H21" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L21" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="M21" s="8"/>
     </row>
@@ -2000,19 +2000,19 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -2021,19 +2021,19 @@
         <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G23" s="8"/>
     </row>

</xml_diff>

<commit_message>
make the acheive ssa split use the denominator of all aims (was previously learners) added a note to make clear why %s might add up to iver 100%
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03AA0741-B64A-4F4A-BBA0-5F03ED59DB39}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{918DC760-AC80-4D89-AAAA-8674A7C96F73}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Update APS source dates in dataText
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{918DC760-AC80-4D89-AAAA-8674A7C96F73}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{3EA00DB4-BDF1-4C0F-8562-3CC5AF44C6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2DE0A0F-7967-43C9-A8DC-6FCEE15FDF81}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -674,10 +674,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">	
-Oct 2022-Sep 2023</t>
-  </si>
-  <si>
     <t>&lt;ol&gt;
   &lt;li&gt;Figures are for 16-64 year olds.&lt;/li&gt;
 &lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
@@ -702,6 +698,10 @@
   </si>
   <si>
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+Jan 2023-Dec 2023</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1182,7 +1182,7 @@
         <v>161</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1194,7 +1194,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>31</v>
@@ -1223,7 +1223,7 @@
         <v>163</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1235,7 +1235,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>32</v>
@@ -1264,7 +1264,7 @@
         <v>164</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1276,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>33</v>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1317,7 +1317,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>34</v>
@@ -1346,7 +1346,7 @@
         <v>162</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1358,7 +1358,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
@@ -1387,7 +1387,7 @@
         <v>165</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1399,7 +1399,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>35</v>
@@ -1428,7 +1428,7 @@
         <v>166</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1440,7 +1440,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>36</v>
@@ -1469,7 +1469,7 @@
         <v>167</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1481,7 +1481,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>37</v>
@@ -1510,16 +1510,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
harris qa (9) ammend job ads data note
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585E6D72-6CB7-4007-9BAD-E71BD6BB9E19}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F9D8F88-5EE8-4A66-B91C-E3064D41B8D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -508,14 +508,6 @@
   </si>
   <si>
     <t>&lt;ol&gt;
-  &lt;li&gt;These statistics should be treated as experimental, as they are still subject to testing the ability to meet user needs.&lt;/li&gt;
-&lt;li&gt;Duplication of adverts can occur when the same job is posted on multiple job boards, or when multiple recruiters advertise the job at the same time.&lt;/li&gt;
-&lt;li&gt;Counts have been rounded to the nearest 5. Totals may not add due to this rounding.&lt;/li&gt;
-&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
   &lt;li&gt;Overall total may not equal the sum of all industries due to rounding and suppression.&lt;/li&gt;
  &lt;li&gt;Unregistered businesses that are not large enough to be registered for VAT or PAYE are not included.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
@@ -678,9 +670,6 @@
     <t>May 2023 data</t>
   </si>
   <si>
-    <t>This data is experimental. ONS are continuing to develop these statistics and aim to publish data regularly. The timescale for the next release has not yet been agreed.</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
   <si>
@@ -730,6 +719,17 @@
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
  &lt;li&gt;Level 4 or above consists of: level 4 (e.g. higher apprenticeship) or above (e.g. higher national diploma, degree apprenticeship, bachelor's, master's, doctorate). &lt;/li&gt;
  &lt;li&gt;From 2022 on qualification level is defined by the National Qualifications Framework (NQF). Before that National Vocational Qualifications (NVQ) is used. &lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). Further data will be published in summer 2024.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;These statistics should be treated as  official statistics in development (previously known as experimental statistics), as they are still subject to testing the ability to meet user needs.&lt;/li&gt;
+&lt;li&gt;Duplication of adverts can occur when the same job is posted on multiple job boards, or when multiple recruiters advertise the job at the same time.&lt;/li&gt;
+&lt;li&gt;Counts have been rounded to the nearest 5. Totals may not add due to this rounding.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
 </sst>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1208,10 +1208,10 @@
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1223,7 +1223,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>31</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1264,7 +1264,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>32</v>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="4" spans="1:13" ht="189" thickBot="1">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1305,7 +1305,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>33</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1346,7 +1346,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>34</v>
@@ -1372,10 +1372,10 @@
     </row>
     <row r="6" spans="1:13" ht="276" thickBot="1">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1387,7 +1387,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
@@ -1405,7 +1405,7 @@
         <v>66</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>68</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1428,7 +1428,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>35</v>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1469,7 +1469,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>36</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1510,7 +1510,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>37</v>
@@ -1534,24 +1534,24 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="203.5" thickBot="1">
+    <row r="10" spans="1:13" ht="218" thickBot="1">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>191</v>
+      <c r="E10" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>38</v>
@@ -1569,7 +1569,7 @@
         <v>81</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>83</v>
@@ -1580,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1592,7 +1592,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>39</v>
@@ -1610,7 +1610,7 @@
         <v>84</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>87</v>
@@ -1621,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1633,7 +1633,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>40</v>
@@ -1662,7 +1662,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1674,7 +1674,7 @@
         <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>41</v>
@@ -1703,19 +1703,19 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>42</v>
@@ -1733,7 +1733,7 @@
         <v>99</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>100</v>
@@ -1744,19 +1744,19 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>43</v>
@@ -1774,7 +1774,7 @@
         <v>101</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>103</v>
@@ -1785,19 +1785,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>44</v>
@@ -1826,19 +1826,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>45</v>
@@ -1864,13 +1864,13 @@
     </row>
     <row r="18" spans="1:13" ht="290.5" thickBot="1">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
@@ -1879,7 +1879,7 @@
         <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>46</v>
@@ -1905,13 +1905,13 @@
     </row>
     <row r="19" spans="1:13" ht="290.5" thickBot="1">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
@@ -1920,28 +1920,28 @@
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="K19" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="263" thickBot="1">
@@ -1952,16 +1952,16 @@
         <v>129</v>
       </c>
       <c r="C20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>47</v>
@@ -1993,16 +1993,16 @@
         <v>129</v>
       </c>
       <c r="C21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>48</v>
@@ -2028,22 +2028,22 @@
     </row>
     <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>128</v>
       </c>
       <c r="C22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" t="s">
         <v>169</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>130</v>
@@ -2070,19 +2070,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -2091,19 +2091,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G24" s="8"/>
     </row>

</xml_diff>

<commit_message>
harris qa (6) add dome data notes to job ads
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F9D8F88-5EE8-4A66-B91C-E3064D41B8D4}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C33E2C-6162-4801-9431-A613144F57FB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -726,9 +726,10 @@
   </si>
   <si>
     <t>&lt;ol&gt;
-  &lt;li&gt;These statistics should be treated as  official statistics in development (previously known as experimental statistics), as they are still subject to testing the ability to meet user needs.&lt;/li&gt;
-&lt;li&gt;Duplication of adverts can occur when the same job is posted on multiple job boards, or when multiple recruiters advertise the job at the same time.&lt;/li&gt;
+  &lt;li&gt;These statistics should be treated as official statistics in development (previously known as experimental statistics), as they are still subject to testing the ability to meet user needs and may be modified in the future.&lt;/li&gt;
 &lt;li&gt;Counts have been rounded to the nearest 5. Totals may not add due to this rounding.&lt;/li&gt;
+&lt;li&gt;Where the same job is identified as being advertised through multiple adverts it is only counted once.&lt;/li&gt;
+&lt;li&gt;The method for allocating jobs to occupations (SOC 2020) is based on the job title of the advert and will be developed further in future releases.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
@@ -1154,7 +1155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1534,7 +1535,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="218" thickBot="1">
+    <row r="10" spans="1:13" ht="247" thickBot="1">
       <c r="A10" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Update references to employment age ranges
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C33E2C-6162-4801-9431-A613144F57FB}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBAB77D5-C672-4195-BC7F-F8B377B7CFE6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="207">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -657,16 +657,6 @@
 &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Employment volumes are for 16-64 year olds.&lt;/li&gt;
-&lt;li&gt;Industry and occupation split volumes are for all ages.&lt;/li&gt;
-&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
-&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
-&lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
-&lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>May 2023 data</t>
   </si>
   <si>
@@ -731,6 +721,30 @@
 &lt;li&gt;Where the same job is identified as being advertised through multiple adverts it is only counted once.&lt;/li&gt;
 &lt;li&gt;The method for allocating jobs to occupations (SOC 2020) is based on the job title of the advert and will be developed further in future releases.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Figures are for all ages (16+).&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Figures are for all ages (16+).&lt;/li&gt;
+&lt;li&gt;The unemployment rate is not the proportion of the total population that is unemployed. It is the proportion of the economically active population (that is, those in work plus those seeking and available to work) that is unemployed.&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Figures are for all ages (16+).&lt;/li&gt;
+&lt;li&gt;Each estimate from the Annual Population Survey carries a margin of error. These are available in the original data via NOMIS. Large margins of error are usually associated with groups with only a small number of respondents. Therefore, please take caution when interpreting data from small subgroups.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
+&lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
 </sst>
@@ -1155,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1212,7 +1226,7 @@
         <v>159</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1253,7 +1267,7 @@
         <v>161</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1289,12 +1303,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="189" thickBot="1">
+    <row r="4" spans="1:13" ht="261.5" thickBot="1">
       <c r="A4" t="s">
         <v>162</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1306,7 +1320,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>33</v>
@@ -1335,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1371,12 +1385,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="276" thickBot="1">
+    <row r="6" spans="1:13" ht="247" thickBot="1">
       <c r="A6" t="s">
         <v>160</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1388,7 +1402,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
@@ -1417,7 +1431,7 @@
         <v>163</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1429,7 +1443,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>35</v>
@@ -1458,7 +1472,7 @@
         <v>164</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1470,7 +1484,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>36</v>
@@ -1499,7 +1513,7 @@
         <v>165</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1540,19 +1554,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>190</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>38</v>
@@ -1868,10 +1882,10 @@
         <v>167</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
@@ -1880,7 +1894,7 @@
         <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>46</v>
@@ -1906,13 +1920,13 @@
     </row>
     <row r="19" spans="1:13" ht="290.5" thickBot="1">
       <c r="A19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>193</v>
-      </c>
       <c r="C19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
@@ -1921,28 +1935,28 @@
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I19" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="K19" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="263" thickBot="1">

</xml_diff>

<commit_message>
Returned to the old learner version of FE breakdown. for provision changed to using the sum of all apps and f&t and cl as denominator because the apps included under 19 and previously we were using the total that didn't have them in added more notes for level around full levels
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/jane8_evans_education_gov_uk/Documents/Documents/Repos/lsip_dashboard/Data/3-2_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{F507649C-394F-469D-AF4E-B1DD86CEE14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBAB77D5-C672-4195-BC7F-F8B377B7CFE6}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="114_{0599F05F-4BCD-4BD7-8E73-6FC6B45720D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{428EF137-C7FF-4A16-A949-62F95A887C1A}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -124,20 +124,9 @@
 Rates are per 100,000 people</t>
   </si>
   <si>
-    <t xml:space="preserve"> Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community.</t>
-  </si>
-  <si>
     <t>Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community.</t>
   </si>
   <si>
-    <t xml:space="preserve">The rates are the number of achievments in AY21/22 per 100,000 of the population. Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The rates are the number of participants in AY21/22 per 100,000 of the population. Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
-</t>
-  </si>
-  <si>
     <t>The employment rate</t>
   </si>
   <si>
@@ -337,9 +326,6 @@
   </si>
   <si>
     <t>Business death rates are</t>
-  </si>
-  <si>
-    <t>The number of FE achievements</t>
   </si>
   <si>
     <t>FE achievements</t>
@@ -746,6 +732,63 @@
 &lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
 &lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
 &lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator shows 19+ further education and skills participation rate per 100,000 population. Further education and skills include apprenticeships and publicly-funded adult learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator shows 19+ further education and skills achievements rate per 100,000 population. Further education and skills include apprenticeships and publicly-funded adult learning, including community learning, delivered by an FE institution, a training provider or within a local community. 
+</t>
+  </si>
+  <si>
+    <t>FE and skills does not includer higher education, unless delivered as part of an apprenticeship programme.
+Apprenticeships are paid jobs that incorporate on-the-job and off-the-job training leading to nationally recognised qualifications.
+Community learning funds a wide range of non-formal courses (e.g. IT or employability skills) and activity targeted at deprived areas or disadvantaged groups. They can be offered by local authorities, colleges, community groups.
+Achievements are the number of learners who successfully complete an individual aim in an academic year.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Achievements included are learners that completed their qualification at any point during the stated academic period.&lt;/li&gt;
+ &lt;li&gt;Learners achieving more than one course will appear only once in totals.&lt;/li&gt;
+ &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Participation includes learners that particpated at any point during the stated academic period.&lt;/li&gt;
+ &lt;li&gt;Learners participating in more than one course will appear only once in the grand total.&lt;/li&gt;
+ &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>The FE achievement rate per 100,000 in</t>
+  </si>
+  <si>
+    <t>The FE participation rate per 100,000 in</t>
+  </si>
+  <si>
+    <t>The number of FE achievements in</t>
+  </si>
+  <si>
+    <t>FE participation in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator shows 19+ further education and skills learner participation. Further education and skills include apprenticeships and publicly-funded adult learning, including community learning, delivered by an FE institution, a training provider or within a local community. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This indicator shows 19+ further education and skills learner achievements. Further education and skills include apprenticeships and publicly-funded adult learning, including community learning, delivered by an FE institution, a training provider or within a local community. </t>
+  </si>
+  <si>
+    <t>The proportion of people qualified at Level 4 or above in</t>
+  </si>
+  <si>
+    <t>The proportion of people qualified at Level 3 or above in</t>
+  </si>
+  <si>
+    <t>The number of online job adverts in</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1213,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1200,33 +1243,33 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" t="s">
         <v>122</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>123</v>
-      </c>
-      <c r="J1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="189" thickBot="1">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1238,36 +1281,36 @@
         <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="189" thickBot="1">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1279,36 +1322,36 @@
         <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="261.5" thickBot="1">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1320,28 +1363,28 @@
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="189" thickBot="1">
@@ -1349,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1361,36 +1404,36 @@
         <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="247" thickBot="1">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1402,36 +1445,36 @@
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="189" thickBot="1">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1443,36 +1486,36 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="189" thickBot="1">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1484,36 +1527,36 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="189" thickBot="1">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1525,28 +1568,28 @@
         <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="247" thickBot="1">
@@ -1554,40 +1597,40 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="145.5" thickBot="1">
@@ -1595,7 +1638,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1607,28 +1650,28 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="319.5" thickBot="1">
@@ -1636,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1648,28 +1691,28 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="319.5" thickBot="1">
@@ -1677,7 +1720,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1689,28 +1732,28 @@
         <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I13" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="363" thickBot="1">
@@ -1718,40 +1761,40 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>213</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="363" thickBot="1">
@@ -1759,40 +1802,40 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>28</v>
+        <v>181</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>102</v>
+        <v>211</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="409.6" thickBot="1">
@@ -1800,40 +1843,40 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>204</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>44</v>
+        <v>208</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="409.6" thickBot="1">
@@ -1841,51 +1884,51 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>45</v>
+        <v>209</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="290.5" thickBot="1">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
@@ -1894,39 +1937,39 @@
         <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>46</v>
+        <v>215</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="290.5" thickBot="1">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
@@ -1935,28 +1978,28 @@
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="L19" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="263" thickBot="1">
@@ -1964,40 +2007,40 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="409.6" thickBot="1">
@@ -2005,78 +2048,78 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="G21" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="409.6" thickBot="1">
       <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="G22" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C22" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E22" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>132</v>
-      </c>
       <c r="L22" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M22" s="8"/>
     </row>
@@ -2085,19 +2128,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -2106,19 +2149,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G24" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add in note on the local skills page about the data quality
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="114_{0599F05F-4BCD-4BD7-8E73-6FC6B45720D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29B2DE84-3BF0-4212-92CB-4C45AF9D1D27}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3411C163-F5C4-415A-AD76-46F36793CD8B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -784,6 +784,13 @@
   </si>
   <si>
     <t>Jul 2023-Jun 2024</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+  ONS published a 
+  &lt;a href="https://osr.statisticsauthority.gov.uk/correspondence/michael-keoghan-to-siobhan-tuohy-smith-request-to-suspend-aps-accreditation/"&gt;response to OSR&lt;/a&gt; about the current quality of Annual Population Survey (APS) (and Labour Force Survey) outputs. ONS asked OSR to temporarily suspend accreditation of all APS-based ONS outputs. There has since been a 
+  &lt;a href="https://osr.statisticsauthority.gov.uk/correspondence/ed-humpherson-to-michael-keoghan-suspension-of-the-accredited-official-statistics-status-for-the-estimates-ons-produces-from-the-annual-population-survey/"&gt;response letter from OSR&lt;/a&gt;. Overall, ONS’ view on the quality of the APS is that while it is robust for national and headline regional estimates, there are concerns with the quality of estimates for smaller segments of the population, such as local authority geographies. ONS will publish an explanatory note later this year providing guidance to users on the quality of current APS and will be used to inform further work ONS is undertaking to improve quality of the survey.
+&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -876,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -895,6 +902,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1211,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1263,7 +1273,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="189" thickBot="1">
+    <row r="2" spans="1:13" ht="409.6" thickBot="1">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -1276,8 +1286,8 @@
       <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
+      <c r="E2" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>180</v>
@@ -1304,7 +1314,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="189" thickBot="1">
+    <row r="3" spans="1:13" ht="409.6" thickBot="1">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -1317,8 +1327,8 @@
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>22</v>
+      <c r="E3" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>180</v>
@@ -1345,7 +1355,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="261.5" thickBot="1">
+    <row r="4" spans="1:13" ht="409.6" thickBot="1">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -1358,8 +1368,8 @@
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
+      <c r="E4" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>195</v>
@@ -1386,7 +1396,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="189" thickBot="1">
+    <row r="5" spans="1:13" ht="409.6" thickBot="1">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1399,8 +1409,8 @@
       <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
+      <c r="E5" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>180</v>
@@ -1427,7 +1437,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="247" thickBot="1">
+    <row r="6" spans="1:13" ht="409.6" thickBot="1">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -1440,8 +1450,8 @@
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
+      <c r="E6" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>196</v>
@@ -1468,7 +1478,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="189" thickBot="1">
+    <row r="7" spans="1:13" ht="409.6" thickBot="1">
       <c r="A7" t="s">
         <v>159</v>
       </c>
@@ -1481,8 +1491,8 @@
       <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>22</v>
+      <c r="E7" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>194</v>
@@ -1509,7 +1519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="189" thickBot="1">
+    <row r="8" spans="1:13" ht="409.6" thickBot="1">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -1522,8 +1532,8 @@
       <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>22</v>
+      <c r="E8" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>194</v>
@@ -1550,7 +1560,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="189" thickBot="1">
+    <row r="9" spans="1:13" ht="409.6" thickBot="1">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -1563,8 +1573,8 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>22</v>
+      <c r="E9" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
adding map comment about missing MCAs
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/rory_burke_education_gov_uk/Documents/GiT Projects/Local Skills Dashboard/Local skills dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67A5692-AB4C-493F-A50D-D32B8BF2C6B5}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47B3EF9-7CA0-4FC4-B1AC-4AF2B456BD10}"/>
   <bookViews>
-    <workbookView xWindow="-15230" yWindow="10690" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -784,10 +784,10 @@
 &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>Nov 2024 data</t>
-  </si>
-  <si>
     <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). Announcement for next data release is tbc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1603,10 +1603,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
adding MCA comment for all other datasets.
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/rory_burke_education_gov_uk/Documents/GiT Projects/Local Skills Dashboard/Local skills dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D47B3EF9-7CA0-4FC4-B1AC-4AF2B456BD10}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69F63ADE-424D-455B-BFBE-E061FFE07689}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -415,9 +415,6 @@
     <t>LaComment</t>
   </si>
   <si>
-    <t>Growth from 2023 to 2035</t>
-  </si>
-  <si>
     <t>Projected employment growth</t>
   </si>
   <si>
@@ -566,12 +563,6 @@
     <t>employment volume share</t>
   </si>
   <si>
-    <t>Dec 2021 - Dec 2022 data</t>
-  </si>
-  <si>
-    <t>AY22/23 data</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2022-23'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -586,9 +577,6 @@
   </si>
   <si>
     <t>L4PlusRate</t>
-  </si>
-  <si>
-    <t>Jan-Dec 2023 data</t>
   </si>
   <si>
     <t>The proportion of people qualified at Level 4 or above</t>
@@ -733,17 +721,11 @@
     <t>Data presented is the baseline projection. Alternative scenarios are available within the published data for UK only.</t>
   </si>
   <si>
-    <t>Jul 2023-Jun 2024</t>
-  </si>
-  <si>
     <t>&lt;p&gt;
   ONS published a 
   &lt;a href="https://osr.statisticsauthority.gov.uk/correspondence/michael-keoghan-to-siobhan-tuohy-smith-request-to-suspend-aps-accreditation/"&gt;response to OSR&lt;/a&gt; about the current quality of Annual Population Survey (APS) (and Labour Force Survey) outputs. ONS asked OSR to temporarily suspend accreditation of all APS-based ONS outputs. There has since been a 
   &lt;a href="https://osr.statisticsauthority.gov.uk/correspondence/ed-humpherson-to-michael-keoghan-suspension-of-the-accredited-official-statistics-status-for-the-estimates-ons-produces-from-the-annual-population-survey/"&gt;response letter from OSR&lt;/a&gt;. Overall, ONS’ view on the quality of the APS is that while it is robust for national and headline regional estimates, there are concerns with the quality of estimates for smaller segments of the population, such as local authority geographies. ONS will publish an explanatory note later this year providing guidance to users on the quality of current APS and will be used to inform further work ONS is undertaking to improve quality of the survey.
 &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Mar 2024 data</t>
   </si>
   <si>
     <t>Destination measures show the percentage of students going to or remaining in an education, apprenticeship or employment destination in the academic year after completing Key Stage 5 studies (usually aged 18). The cohort of learners used in the metrics here completed in AY21/22.</t>
@@ -788,6 +770,24 @@
   </si>
   <si>
     <t xml:space="preserve">Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul 2023-Jun 2024.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar 2024 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 2021 - Dec 2022 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AY22/23 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan-Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth from 2023 to 2035.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="2" spans="1:13" ht="409.6" thickBot="1">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1284,16 +1284,16 @@
         <v>19</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>48</v>
@@ -1313,10 +1313,10 @@
     </row>
     <row r="3" spans="1:13" ht="409.6" thickBot="1">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1325,16 +1325,16 @@
         <v>19</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>53</v>
@@ -1354,10 +1354,10 @@
     </row>
     <row r="4" spans="1:13" ht="409.6" thickBot="1">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1366,16 +1366,16 @@
         <v>19</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>48</v>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1407,16 +1407,16 @@
         <v>19</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>60</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="6" spans="1:13" ht="409.6" thickBot="1">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1448,16 +1448,16 @@
         <v>19</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>64</v>
@@ -1469,7 +1469,7 @@
         <v>63</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>65</v>
@@ -1477,10 +1477,10 @@
     </row>
     <row r="7" spans="1:13" ht="409.6" thickBot="1">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1489,16 +1489,16 @@
         <v>19</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>67</v>
@@ -1518,10 +1518,10 @@
     </row>
     <row r="8" spans="1:13" ht="409.6" thickBot="1">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1530,16 +1530,16 @@
         <v>19</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>71</v>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="9" spans="1:13" ht="409.6" thickBot="1">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1571,16 +1571,16 @@
         <v>19</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>75</v>
@@ -1603,28 +1603,28 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>79</v>
@@ -1633,7 +1633,7 @@
         <v>78</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>80</v>
@@ -1644,7 +1644,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1656,13 +1656,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>82</v>
@@ -1674,7 +1674,7 @@
         <v>81</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>84</v>
@@ -1685,7 +1685,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>168</v>
+        <v>212</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1697,13 +1697,13 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>86</v>
@@ -1726,7 +1726,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>212</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1738,13 +1738,13 @@
         <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>91</v>
@@ -1767,28 +1767,28 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>95</v>
@@ -1797,7 +1797,7 @@
         <v>95</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>96</v>
@@ -1808,28 +1808,28 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>98</v>
@@ -1838,7 +1838,7 @@
         <v>97</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>99</v>
@@ -1849,28 +1849,28 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>101</v>
@@ -1890,28 +1890,28 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D17" t="s">
-        <v>170</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>104</v>
@@ -1928,13 +1928,13 @@
     </row>
     <row r="18" spans="1:13" ht="290.5" thickBot="1">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
@@ -1943,16 +1943,16 @@
         <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>107</v>
@@ -1969,13 +1969,13 @@
     </row>
     <row r="19" spans="1:13" ht="290.5" thickBot="1">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
@@ -1984,28 +1984,28 @@
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="L19" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="263" thickBot="1">
@@ -2013,25 +2013,25 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>44</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>44</v>
@@ -2054,25 +2054,25 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>45</v>
@@ -2092,40 +2092,40 @@
     </row>
     <row r="22" spans="1:13" ht="334" thickBot="1">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>124</v>
+        <v>215</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E22" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>64</v>
       </c>
       <c r="J22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="M22" s="8"/>
     </row>
@@ -2134,19 +2134,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -2155,19 +2155,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G24" s="8"/>
     </row>

</xml_diff>

<commit_message>
removed whitespace which should remove double full stop on MCA message.
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/rory_burke_education_gov_uk/Documents/GiT Projects/Local Skills Dashboard/Local skills dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69F63ADE-424D-455B-BFBE-E061FFE07689}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AAC6A40-A8A4-4AB4-A7B2-174FFE8D5978}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -769,25 +769,25 @@
     <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). Announcement for next data release is tbc.</t>
   </si>
   <si>
-    <t xml:space="preserve">Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jul 2023-Jun 2024.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mar 2024 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 2021 - Dec 2022 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AY22/23 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan-Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growth from 2023 to 2035.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on. </t>
+    <t>Jul 2023-Jun 2024.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+  </si>
+  <si>
+    <t>Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+  </si>
+  <si>
+    <t>Mar 2024 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+  </si>
+  <si>
+    <t>Dec 2021 - Dec 2022 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+  </si>
+  <si>
+    <t>AY22/23 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+  </si>
+  <si>
+    <t>Jan-Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+  </si>
+  <si>
+    <t>Growth from 2023 to 2035.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1275,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1316,7 +1316,7 @@
         <v>155</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1357,7 +1357,7 @@
         <v>156</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1439,7 +1439,7 @@
         <v>154</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1480,7 +1480,7 @@
         <v>157</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1521,7 +1521,7 @@
         <v>158</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1562,7 +1562,7 @@
         <v>159</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1603,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
trying to fix double fullstop by removing the fullstop completely from datatext
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/rory_burke_education_gov_uk/Documents/GiT Projects/Local Skills Dashboard/Local skills dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AAC6A40-A8A4-4AB4-A7B2-174FFE8D5978}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{842D1F76-F660-4041-A684-7CDB08B97A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{695CFA0D-E5BC-4D82-A8FB-F22346A8277B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -769,25 +769,25 @@
     <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). Announcement for next data release is tbc.</t>
   </si>
   <si>
-    <t>Jul 2023-Jun 2024.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
-  </si>
-  <si>
-    <t>Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
-  </si>
-  <si>
-    <t>Mar 2024 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
-  </si>
-  <si>
-    <t>Dec 2021 - Dec 2022 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
-  </si>
-  <si>
-    <t>AY22/23 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
-  </si>
-  <si>
-    <t>Jan-Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
-  </si>
-  <si>
-    <t>Growth from 2023 to 2035.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on.</t>
+    <t>Jul 2023-Jun 2024.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
+  </si>
+  <si>
+    <t>Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
+  </si>
+  <si>
+    <t>Mar 2024 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
+  </si>
+  <si>
+    <t>Dec 2021 - Dec 2022 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
+  </si>
+  <si>
+    <t>AY22/23 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
+  </si>
+  <si>
+    <t>Jan-Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
+  </si>
+  <si>
+    <t>Growth from 2023 to 2035.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Updated some text that refrenced the old MCA boundaries
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{C632E5F5-1B09-41BB-888F-70ACD4C23F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AE9E043-FAA5-44DD-B33F-7C0F8E128154}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C632E5F5-1B09-41BB-888F-70ACD4C23F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAD3A1B-E086-4B2B-B703-834DCEC36619}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -769,31 +769,31 @@
     <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). Announcement for next data release is tbc.</t>
   </si>
   <si>
-    <t>Nov 2024 data. North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>Mar 2024 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>AY22/23 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>Jan-Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>Growth from 2023 to 2035.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>Dec 2022 - Dec 2023 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>Oct 2023-Sep 2024.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
-    <t>AY23/24 data.  North East and North of Tyne MCA have temporarily been removed, on account of North of Tyne being integrated into North East from now on</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/b930498d-b4f0-416d-a086-7acee1be8179'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oct 2023-Sep 2024. </t>
+  </si>
+  <si>
+    <t>Nov 2024 data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar 2024 data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 2022 - Dec 2023 data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AY23/24 data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan-Dec 2023 data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AY22/23 data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth from 2023 to 2035. </t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1281,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1322,7 +1322,7 @@
         <v>155</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1363,7 +1363,7 @@
         <v>156</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1445,7 +1445,7 @@
         <v>154</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1486,7 +1486,7 @@
         <v>157</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1527,7 +1527,7 @@
         <v>158</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1568,7 +1568,7 @@
         <v>159</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1609,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>208</v>
@@ -1650,7 +1650,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1691,7 +1691,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1732,7 +1732,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1773,13 +1773,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>194</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -1814,13 +1814,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
@@ -1855,13 +1855,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>186</v>
@@ -1896,13 +1896,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>184</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>186</v>
@@ -1937,7 +1937,7 @@
         <v>161</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
         <v>177</v>
@@ -1978,7 +1978,7 @@
         <v>170</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s">
         <v>177</v>
@@ -2019,7 +2019,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C20" t="s">
         <v>202</v>
@@ -2060,7 +2060,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C21" t="s">
         <v>201</v>
@@ -2101,7 +2101,7 @@
         <v>160</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -2140,7 +2140,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -2161,7 +2161,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Remove extraneous full stop
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{C632E5F5-1B09-41BB-888F-70ACD4C23F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86B43CCA-65D8-4352-86F6-924305AD290B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{C632E5F5-1B09-41BB-888F-70ACD4C23F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BC98B2-BD65-43E7-9F83-9554C3468CC1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -772,9 +772,6 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/b930498d-b4f0-416d-a086-7acee1be8179'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Nov 2024 data.</t>
-  </si>
-  <si>
     <t>Oct 2023-Sep 2024</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>Growth from 2023 to 2035</t>
+  </si>
+  <si>
+    <t>Nov 2024 data</t>
   </si>
 </sst>
 </file>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B18" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1281,7 +1281,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1322,7 +1322,7 @@
         <v>155</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1363,7 +1363,7 @@
         <v>156</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1445,7 +1445,7 @@
         <v>154</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1486,7 +1486,7 @@
         <v>157</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1527,7 +1527,7 @@
         <v>158</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1568,7 +1568,7 @@
         <v>159</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1609,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>208</v>
@@ -1650,7 +1650,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1691,7 +1691,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1732,7 +1732,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1773,7 +1773,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>194</v>
@@ -1814,7 +1814,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>193</v>
@@ -1855,7 +1855,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>185</v>
@@ -1896,7 +1896,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>184</v>
@@ -1937,7 +1937,7 @@
         <v>161</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C18" t="s">
         <v>177</v>
@@ -1978,7 +1978,7 @@
         <v>170</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
         <v>177</v>
@@ -2019,7 +2019,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" t="s">
         <v>202</v>
@@ -2060,7 +2060,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
         <v>201</v>
@@ -2101,7 +2101,7 @@
         <v>160</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -2140,7 +2140,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -2161,7 +2161,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update job ads subtitle Update version control Run tests
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-2_dataText\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D82A07-7D31-4EBE-8D57-8A2D9B394592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A3D82A07-7D31-4EBE-8D57-8A2D9B394592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{500C7C74-4AB0-4F48-A817-0B8417DEFBA9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -760,9 +760,6 @@
 &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). Announcement for next data release is tbc.</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/b930498d-b4f0-416d-a086-7acee1be8179'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>Jan-Dec 2024 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These statistics should be treated as official statistics in development (previously known as experimental statistics). </t>
   </si>
 </sst>
 </file>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1283,7 +1283,7 @@
         <v>153</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1324,7 +1324,7 @@
         <v>155</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1365,7 +1365,7 @@
         <v>156</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1406,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1447,7 +1447,7 @@
         <v>154</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1488,7 +1488,7 @@
         <v>157</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1529,7 +1529,7 @@
         <v>158</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1570,7 +1570,7 @@
         <v>159</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1611,10 +1611,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>169</v>
@@ -1652,7 +1652,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1734,7 +1734,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1775,13 +1775,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>194</v>
       </c>
       <c r="D14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -1816,13 +1816,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
@@ -1857,13 +1857,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>186</v>
@@ -1898,13 +1898,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>184</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>186</v>
@@ -1939,7 +1939,7 @@
         <v>161</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s">
         <v>177</v>
@@ -1980,7 +1980,7 @@
         <v>170</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
         <v>177</v>
@@ -2021,13 +2021,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
         <v>202</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>203</v>
@@ -2062,13 +2062,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
         <v>201</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>204</v>
@@ -2103,7 +2103,7 @@
         <v>160</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -2142,7 +2142,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -2163,7 +2163,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update skills imperative metric to growth from 2024 (was 2023). Changed label on time chart for skills imperative to Annual growth
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-2_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{A3D82A07-7D31-4EBE-8D57-8A2D9B394592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5705A226-9390-4C7B-97C4-788CB51D7B0A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A84076-B629-42A7-BA34-57CD223AA1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="5040" yWindow="20" windowWidth="15310" windowHeight="14300" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -416,9 +416,6 @@
   </si>
   <si>
     <t>Projected employment growth</t>
-  </si>
-  <si>
-    <t>Projected employment growth from 2023 to 2035</t>
   </si>
   <si>
     <t>projected employment volume changes</t>
@@ -766,9 +763,6 @@
     <t>AY22/23 data</t>
   </si>
   <si>
-    <t>Growth from 2023 to 2035</t>
-  </si>
-  <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/find-statistics/key-stage-4-destination-measures/2022-23'&gt;Key stage 4 destination measures&lt;/a&gt;</t>
   </si>
   <si>
@@ -793,6 +787,9 @@
   </si>
   <si>
     <t>Apr 2024 - Mar 2025</t>
+  </si>
+  <si>
+    <t>Growth from 2024 to 2035</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1279,10 +1276,10 @@
     </row>
     <row r="2" spans="1:13" ht="409.6" thickBot="1">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1291,16 +1288,16 @@
         <v>19</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>48</v>
@@ -1320,10 +1317,10 @@
     </row>
     <row r="3" spans="1:13" ht="409.6" thickBot="1">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1332,16 +1329,16 @@
         <v>19</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>53</v>
@@ -1361,10 +1358,10 @@
     </row>
     <row r="4" spans="1:13" ht="409.6" thickBot="1">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1373,16 +1370,16 @@
         <v>19</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>48</v>
@@ -1405,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1414,16 +1411,16 @@
         <v>19</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>60</v>
@@ -1443,10 +1440,10 @@
     </row>
     <row r="6" spans="1:13" ht="409.6" thickBot="1">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1455,16 +1452,16 @@
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>64</v>
@@ -1476,7 +1473,7 @@
         <v>63</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>65</v>
@@ -1484,10 +1481,10 @@
     </row>
     <row r="7" spans="1:13" ht="409.6" thickBot="1">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1496,16 +1493,16 @@
         <v>19</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>67</v>
@@ -1525,10 +1522,10 @@
     </row>
     <row r="8" spans="1:13" ht="409.6" thickBot="1">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1537,16 +1534,16 @@
         <v>19</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>71</v>
@@ -1566,10 +1563,10 @@
     </row>
     <row r="9" spans="1:13" ht="409.6" thickBot="1">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1578,16 +1575,16 @@
         <v>19</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>75</v>
@@ -1610,28 +1607,28 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>79</v>
@@ -1640,7 +1637,7 @@
         <v>78</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>80</v>
@@ -1651,7 +1648,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1663,13 +1660,13 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>82</v>
@@ -1681,7 +1678,7 @@
         <v>81</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>84</v>
@@ -1692,7 +1689,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1704,13 +1701,13 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>86</v>
@@ -1733,7 +1730,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1745,13 +1742,13 @@
         <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>91</v>
@@ -1774,28 +1771,28 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>95</v>
@@ -1804,7 +1801,7 @@
         <v>95</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>96</v>
@@ -1815,28 +1812,28 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>98</v>
@@ -1845,7 +1842,7 @@
         <v>97</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>99</v>
@@ -1856,28 +1853,28 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D16" t="s">
-        <v>205</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>101</v>
@@ -1897,28 +1894,28 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>104</v>
@@ -1935,13 +1932,13 @@
     </row>
     <row r="18" spans="1:13" ht="290.5" thickBot="1">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>19</v>
@@ -1950,16 +1947,16 @@
         <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>43</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>107</v>
@@ -1976,13 +1973,13 @@
     </row>
     <row r="19" spans="1:13" ht="290.5" thickBot="1">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>19</v>
@@ -1991,28 +1988,28 @@
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I19" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="K19" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="263" thickBot="1">
@@ -2020,25 +2017,25 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>44</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>44</v>
@@ -2061,25 +2058,25 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>45</v>
@@ -2099,40 +2096,40 @@
     </row>
     <row r="22" spans="1:13" ht="334" thickBot="1">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>124</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>64</v>
       </c>
       <c r="J22" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="M22" s="8"/>
     </row>
@@ -2141,19 +2138,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G23" s="8"/>
     </row>
@@ -2162,19 +2159,19 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G24" s="8"/>
     </row>

</xml_diff>

<commit_message>
Update to the latest LSIP geographies: Update all data to allign with the new LSIP geographies, usually by applying the new lookup. Where data is published at LSIP level (skills imperative and FE data) use the published data where the LSIP geography has not changed. Else, for FE build up from LAs, for skills imp, show blank data and add error messages. Also some work to allign name of LSIPs to the new names. In the case of NOMIS data, new "user defined" geographies have been created for the LSIPs and the London MCA. New LSIP boundaries are created by combining LA boundaries (as is the London MCA boundary). There have been a few instances of code cleaning to get rid of some old LEP references. There has been some additional code cleaning to remove warnings from running the extract and load process. Removed a lot of the raw skills imp files that are no longer used (LEPs and some LSIPs). Delete data archive (no longer used)
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmt1pr-dhfs01\Personal\MMEHTA4\Repos\lsip_dashboard\Data\3-2_dataText\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594FBCF-5455-49E4-A10C-326E0EA0A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5594FBCF-5455-49E4-A10C-326E0EA0A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F1D1A83-C468-4798-AE14-1519C78973B7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="218">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -790,6 +790,9 @@
   </si>
   <si>
     <t>July 2025 data</t>
+  </si>
+  <si>
+    <t>Growth from 2024 to 2035. The LSIP boundaries have changed since this data was published so some LSIPs no longer have data</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1225,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -2097,7 +2102,7 @@
         <v>159</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Add in new MCAs. This involved: a) getting new look-up b) creating boundaries for the new areas c) adjusting code throughout to match the new lookup Add error statements to charts when: a) a london LSIP and vacancies (no data) b) a changed area (LSIPs) or new area (MCAs) and skills imp data
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5594FBCF-5455-49E4-A10C-326E0EA0A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F1D1A83-C468-4798-AE14-1519C78973B7}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{5594FBCF-5455-49E4-A10C-326E0EA0A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4372C73-E7AE-46CD-8640-C17D5EA8051E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -792,7 +792,7 @@
     <t>July 2025 data</t>
   </si>
   <si>
-    <t>Growth from 2024 to 2035. The LSIP boundaries have changed since this data was published so some LSIPs no longer have data</t>
+    <t>Growth from 2024 to 2035. The LSIP boundaries have changed and new MCAs have been created since this data was published so some areas no longer have data</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Root out all mentioned of MCA and switch to CA.
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{5594FBCF-5455-49E4-A10C-326E0EA0A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4372C73-E7AE-46CD-8640-C17D5EA8051E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5594FBCF-5455-49E4-A10C-326E0EA0A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DBC51A-6437-4170-94D6-33A6417FFAD3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -792,7 +792,7 @@
     <t>July 2025 data</t>
   </si>
   <si>
-    <t>Growth from 2024 to 2035. The LSIP boundaries have changed and new MCAs have been created since this data was published so some areas no longer have data</t>
+    <t>Growth from 2024 to 2035. The LSIP boundaries have changed and new CAs have been created since this data was published so some areas no longer have data</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Update data text tables. Round breakdown to 4 dp to avoid rounding errors.
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/3-2_dataText/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-2_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{A7EED92E-FFBB-48EE-A880-A61DC579FD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{655495D2-3DF7-4328-A444-B9AC2894413F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AD010C-A709-4448-9D66-68B90B2D9F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -716,32 +716,6 @@
 &lt;/p&gt;</t>
   </si>
   <si>
-    <t>Destination measures show the percentage of students going to or remaining in an education, apprenticeship or employment destination in the academic year after completing Key Stage 4 studies (usually aged between 14 to 16). The cohort of learners used in the metrics here completed in AY21/22.
-A sustained destination is a count of young people recorded as having sustained participation (education and employment) for a 6 month period in the destination year.
-This means attending for all of the first two terms of the academic year (e.g. October 2021 to March 2022) at one or more education providers; spending 5 of the 6 months in employment or a combination of the two.
-A sustained apprenticeship is recorded when 6 months continuous participation is recorded at any point in the destination year (between August 2021 and July 2022).
-Not recorded includes pupils who were captured in the destination source data but who failed to meet the sustained participation criteria.
-Unknown (activity not captured): The student was not found to have any participation in education, apprenticeship or employment nor recorded as receiving out-of-work benefits at any point in the year. This also includes not being recorded by their Local Authority as NEET (not engaged in education, employment or training).</t>
-  </si>
-  <si>
-    <t>Destination measures show the percentage of students going to or remaining in an education, apprenticeship or employment destination in the academic year after completing Key Stage 5 studies (usually aged 18). The cohort of learners used in the metrics here completed in AY21/22.
-A sustained destination is a count of young people recorded as having sustained participation (education and employment) for a 6 month period in the destination year.
-This means attending for all of the first two terms of the academic year (e.g. October 2021 to March 2022) at one or more education providers; spending 5 of the 6 months in employment or a combination of the two.
-A sustained apprenticeship is recorded when 6 months continuous participation is recorded at any point in the destination year (between August 2021 and July 2022).
-Not recorded includes pupils who were captured in the destination source data but who failed to meet the sustained participation criteria.
-Unknown (activity not captured): The student was not found to have any participation in education, apprenticeship or employment nor recorded as receiving out-of-work benefits at any point in the year. This also includes not being recorded by their Local Authority as NEET (not engaged in education, employment or training).</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-&lt;li&gt;The definition of when a student is at the end of 16 to 18 study has changed last year and comparisons to previous cohorts should be treated with caution. Students are included in this statistical release when they reach the end of 16 to 18 study. The ‘trigger’ rules for deciding when this happens changed in 2020/21. Further details can be found in the &lt;a href = https://explore-education-statistics.service.gov.uk/find-statistics/16-18-destination-measures'&gt;publication&lt;/a&gt;.&lt;/li&gt;
-&lt;li&gt;There was no checking exercise for this cohort of students. The checking exercise ordinarily allows schools and colleges to confirm whether the students we report are at end of 16 to 18 study. This means that this data may not accurately represent whether students were at the end of 16 to 18 study in 2020/21.&lt;/li&gt;
-  &lt;li&gt;Data based on destinations of state-funded mainstream schools and colleges.&lt;/li&gt;
- &lt;li&gt;There is no double counting across destinations, a young person is reported in one destination category only.&lt;/li&gt;
- &lt;li&gt;If a student is registered as being in education and an apprenticeship, it is recorded as a sustained education and if a student is registered in employment along with an apprenticeship or in education, it is recorded as sustained employment.&lt;/li&gt;
-&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/b930498d-b4f0-416d-a086-7acee1be8179'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -793,6 +767,30 @@
   </si>
   <si>
     <t>Destination measures show the percentage of students going to or remaining in an education, apprenticeship or employment destination in the academic year after completing Key Stage 5 studies (usually aged 18). The cohort of learners used in the metrics here completed in AY22/23.</t>
+  </si>
+  <si>
+    <t>Destination measures show the percentage of students going to or remaining in an education, apprenticeship or employment destination in the academic year after completing Key Stage 4 studies (usually aged between 14 to 16). The cohort of learners used in the metrics here completed in AY22/23.
+A sustained destination is a count of young people recorded as having sustained participation (education and employment) for a 6 month period in the destination year.
+This means attending for all of the first two terms of the academic year (e.g. October 2022 to March 2023) at one or more education providers; spending 5 of the 6 months in employment or a combination of the two.
+A sustained apprenticeship is recorded when 6 months continuous participation is recorded at any point in the destination year (between August 2022 and July 2023).
+Not recorded includes pupils who were captured in the destination source data but who failed to meet the sustained participation criteria.
+Unknown (activity not captured): The student was not found to have any participation in education, apprenticeship or employment nor recorded as receiving out-of-work benefits at any point in the year. This also includes not being recorded by their Local Authority as NEET (not engaged in education, employment or training).</t>
+  </si>
+  <si>
+    <t>Destination measures show the percentage of students going to or remaining in an education, apprenticeship or employment destination in the academic year after completing Key Stage 5 studies (usually aged 18). The cohort of learners used in the metrics here completed in AY22/23.
+A sustained destination is a count of young people recorded as having sustained participation (education and employment) for a 6 month period in the destination year.
+This means attending for all of the first two terms of the academic year (e.g. October 2022 to March 2023) at one or more education providers; spending 5 of the 6 months in employment or a combination of the two.
+A sustained apprenticeship is recorded when 6 months continuous participation is recorded at any point in the destination year (between August 2022 and July 2023).
+Not recorded includes pupils who were captured in the destination source data but who failed to meet the sustained participation criteria.
+Unknown (activity not captured): The student was not found to have any participation in education, apprenticeship or employment nor recorded as receiving out-of-work benefits at any point in the year. This also includes not being recorded by their Local Authority as NEET (not engaged in education, employment or training).</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Data based on destinations of state-funded mainstream schools and colleges.&lt;/li&gt;
+ &lt;li&gt;There is no double counting across destinations, a young person is reported in one destination category only.&lt;/li&gt;
+ &lt;li&gt;If a student is registered as being in education and an apprenticeship, it is recorded as a sustained education and if a student is registered in employment along with an apprenticeship or in education, it is recorded as sustained employment.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;/ol&gt;</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1282,7 +1280,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1323,7 +1321,7 @@
         <v>154</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1364,7 +1362,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1405,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1446,7 +1444,7 @@
         <v>153</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1487,7 +1485,7 @@
         <v>156</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1528,7 +1526,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1569,7 +1567,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1610,10 +1608,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>168</v>
@@ -1622,7 +1620,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>35</v>
@@ -1651,7 +1649,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1692,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1733,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1774,13 +1772,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>18</v>
@@ -1815,13 +1813,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>18</v>
@@ -1856,13 +1854,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>184</v>
@@ -1897,13 +1895,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>184</v>
@@ -1938,7 +1936,7 @@
         <v>160</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
         <v>176</v>
@@ -1979,7 +1977,7 @@
         <v>169</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C19" t="s">
         <v>176</v>
@@ -2020,16 +2018,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C20" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>150</v>
@@ -2056,24 +2054,24 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="409.6" thickBot="1">
+    <row r="21" spans="1:13" ht="254" thickBot="1">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>45</v>
@@ -2102,7 +2100,7 @@
         <v>159</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -2126,7 +2124,7 @@
         <v>64</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>125</v>
@@ -2141,7 +2139,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -2162,7 +2160,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Add note on the missing job ads data. Update version control.
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-2_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D71E6F-851C-4896-B1FB-8161B364847D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5420C27-934F-49A7-B748-DA5054C86ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -737,9 +737,6 @@
     <t>Jan-Dec 2024 data</t>
   </si>
   <si>
-    <t xml:space="preserve">These statistics should be treated as official statistics in development (previously known as experimental statistics). </t>
-  </si>
-  <si>
     <t>&lt;ol&gt;
   &lt;li&gt;These statistics should be treated as official statistics in development (previously known as experimental statistics), as they are still subject to testing the ability to meet user needs and may be modified in the future.&lt;/li&gt;
 &lt;li&gt;Where the same job is identified as being advertised through multiple adverts it is only counted once.&lt;/li&gt;
@@ -791,6 +788,9 @@
   </si>
   <si>
     <t>Jul 2024 - Jun 2025</t>
+  </si>
+  <si>
+    <t>These statistics should be treated as official statistics in development (previously known as experimental statistics). ONS have temporarily paused publication of the snapshot metric for online job adverts so the latest data available covers up to July 2025. More up to date data on new adverts is still available directly from the  &lt;a href="https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbystandardoccupationclassificationsoc2020uk"&gt;ONS website&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1278,7 +1278,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1319,7 +1319,7 @@
         <v>154</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1360,7 +1360,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1401,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1442,7 +1442,7 @@
         <v>153</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1483,7 +1483,7 @@
         <v>156</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1524,7 +1524,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1565,7 +1565,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1606,10 +1606,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>168</v>
@@ -1618,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>35</v>
@@ -1647,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -2019,13 +2019,13 @@
         <v>201</v>
       </c>
       <c r="C20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>203</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>150</v>
@@ -2060,16 +2060,16 @@
         <v>201</v>
       </c>
       <c r="C21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>204</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>45</v>
@@ -2098,7 +2098,7 @@
         <v>159</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -2122,7 +2122,7 @@
         <v>64</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Add missing FE footnote text
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jevans8\Repos\lsip_dashboard\Data\3-2_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42F8BDB-18D2-4A8E-9865-2855133E95DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA23BE7-D657-4EF6-B0A9-006B1484A2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="219">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -777,12 +777,6 @@
   <si>
     <t xml:space="preserve">This indicator shows 19+ further education and skills achievements rate per 100,000 population. Further education and skills include apprenticeships and publicly-funded adult learning, including tailored learning, delivered by an FE institution, a training provider or within a local community. 
 </t>
-  </si>
-  <si>
-    <t>FE and skills does not includer higher education, unless delivered as part of an apprenticeship programme.
-Apprenticeships are paid jobs that incorporate on-the-job and off-the-job training leading to nationally recognised qualifications.
-Tailored learning is primarily non-qualification based provision that is tailored to the skills needs of the learners, employers and local communities.
-Achievements are the number of learners who successfully complete an individual aim in an academic year.</t>
   </si>
   <si>
     <t xml:space="preserve">This indicator shows 19+ further education and skills participation rate per 100,000 population. Further education and skills include apprenticeships and publicly-funded adult learning, including tailored learning, delivered by an FE institution, a training provider or within a local community. 
@@ -1236,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1791,7 +1785,7 @@
         <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>213</v>
@@ -1832,13 +1826,13 @@
         <v>212</v>
       </c>
       <c r="D15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>40</v>
@@ -1873,10 +1867,10 @@
         <v>214</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>182</v>
@@ -1911,16 +1905,16 @@
         <v>211</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" t="s">
         <v>216</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>42</v>
@@ -2026,7 +2020,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="272" thickBot="1">
+    <row r="20" spans="1:13" ht="263" thickBot="1">
       <c r="A20" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Add fotnote to explain FE rounding errors
</commit_message>
<xml_diff>
--- a/Data/3-2_dataText/dataText.xlsx
+++ b/Data/3-2_dataText/dataText.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jevans8\Repos\lsip_dashboard\Data\3-2_dataText\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA23BE7-D657-4EF6-B0A9-006B1484A2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC4C16-EB78-4779-978A-367C83BDA8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E004AAF5-AC7D-409D-877C-9EBD23056743}"/>
   </bookViews>
   <sheets>
     <sheet name="dataText" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="220">
   <si>
     <t>inactiveRate</t>
   </si>
@@ -636,14 +636,6 @@
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;li&gt;Standard Occupational Classification 2020 (SOC2020).&lt;/li&gt;
 &lt;li&gt;Industry groups are Standard Industrial Classification: SIC 2007.&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;
-  &lt;li&gt;Achievements included are learners that completed their qualification at any point during the stated academic period.&lt;/li&gt;
- &lt;li&gt;Learners achieving more than one course will appear only once in totals.&lt;/li&gt;
- &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
-&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
   <si>
@@ -786,20 +778,39 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/data-set/1977cdbc-7eae-4257-a8c9-3281bb2dbfa9'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
+    <t>Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including tailored learning, delivered by an FE institution, a training provider or within a local community.
+FE and skills does not includer higher education, unless delivered as part of an apprenticeship programme.
+Apprenticeships are paid jobs that incorporate on-the-job and off-the-job training leading to nationally recognised qualifications.
+Tailored learning is primarily non-qualification based provision that is tailored to the skills needs of the learners, employers and local communities.
+Participation is the number of learners who attended at least one day on a learning aim.</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Total achievements is the count of learners that completed their qualification at any point during the stated academic period.&lt;/li&gt;
+ &lt;li&gt;Learners achieving more than one course will appear only once in the grand total.&lt;/li&gt;
+ &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;li&gt;Figures for newly formed CAs have been calculated from Local Authority data to create a back series. There may be small differences to the published data for these geographies due to rounding errors.&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
     <t>&lt;ol&gt;
   &lt;li&gt;Total participation is a count of the number of learners who attended at least one day on a learning aim.&lt;/li&gt;
  &lt;li&gt;A learner who is studying more than one learning aim at different levels or different community learning purpose types, is counted once against each level or type.&lt;/li&gt; 
 &lt;li&gt;A learner is counted only once in any total (e.g. national) count of participation, regardless of how many different learning aims they have.&lt;/li&gt;
  &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
 &lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;li&gt;Figures for newly formed CAs have been calculated from Local Authority data to create a back series. There may be small differences to the published data for these geographies due to rounding errors.&lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>Further education and skills include all age apprenticeships and publicly-funded adult (19+) learning, including tailored learning, delivered by an FE institution, a training provider or within a local community.
-FE and skills does not includer higher education, unless delivered as part of an apprenticeship programme.
-Apprenticeships are paid jobs that incorporate on-the-job and off-the-job training leading to nationally recognised qualifications.
-Tailored learning is primarily non-qualification based provision that is tailored to the skills needs of the learners, employers and local communities.
-Participation is the number of learners who attended at least one day on a learning aim.</t>
+    <t>&lt;ol&gt;
+  &lt;li&gt;Achievements included are learners that completed their qualification at any point during the stated academic period.&lt;/li&gt;
+ &lt;li&gt;Learners achieving more than one course will appear only once in totals.&lt;/li&gt;
+ &lt;li&gt;Years shown represent academic years.&lt;/li&gt;
+&lt;li&gt;Use caution when interpreting this data. A difference between subgroups does not necessarily imply any causality. There could be other contributing factors at work.&lt;/li&gt;
+&lt;li&gt;Figures for newly formed CAs have been calculated from Local Authority data to create a back series. There may be small differences to the published data for these geographies due to rounding errors.&lt;/li&gt;
+&lt;/ol&gt;</t>
   </si>
 </sst>
 </file>
@@ -1230,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D33D53-EEC7-4B18-8C67-5F9034426AB5}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1287,7 +1298,7 @@
         <v>152</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>22</v>
@@ -1296,7 +1307,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>167</v>
@@ -1328,7 +1339,7 @@
         <v>154</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -1337,7 +1348,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>167</v>
@@ -1369,7 +1380,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>22</v>
@@ -1378,7 +1389,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>180</v>
@@ -1410,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>22</v>
@@ -1419,7 +1430,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>167</v>
@@ -1451,7 +1462,7 @@
         <v>153</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -1460,7 +1471,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>181</v>
@@ -1492,7 +1503,7 @@
         <v>156</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1501,7 +1512,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>179</v>
@@ -1533,7 +1544,7 @@
         <v>157</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>22</v>
@@ -1542,7 +1553,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>179</v>
@@ -1574,7 +1585,7 @@
         <v>158</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>22</v>
@@ -1583,7 +1594,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>167</v>
@@ -1615,10 +1626,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>168</v>
@@ -1627,7 +1638,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>35</v>
@@ -1636,7 +1647,7 @@
         <v>135</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>79</v>
@@ -1656,7 +1667,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>23</v>
@@ -1697,7 +1708,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>23</v>
@@ -1738,7 +1749,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
@@ -1779,19 +1790,19 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D14" t="s">
-        <v>216</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>39</v>
@@ -1800,7 +1811,7 @@
         <v>139</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>95</v>
@@ -1820,19 +1831,19 @@
         <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="D15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>40</v>
@@ -1841,7 +1852,7 @@
         <v>140</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>98</v>
@@ -1861,19 +1872,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>41</v>
@@ -1882,7 +1893,7 @@
         <v>141</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>101</v>
@@ -1902,19 +1913,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D17" t="s">
         <v>215</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>42</v>
@@ -1923,7 +1934,7 @@
         <v>142</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>104</v>
@@ -1943,7 +1954,7 @@
         <v>160</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
         <v>176</v>
@@ -1964,7 +1975,7 @@
         <v>143</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>107</v>
@@ -1984,7 +1995,7 @@
         <v>169</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
         <v>176</v>
@@ -2005,7 +2016,7 @@
         <v>171</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>172</v>
@@ -2025,16 +2036,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>150</v>
@@ -2066,19 +2077,19 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>45</v>
@@ -2107,7 +2118,7 @@
         <v>159</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -2116,10 +2127,10 @@
         <v>151</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>124</v>
@@ -2131,7 +2142,7 @@
         <v>64</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>125</v>
@@ -2146,7 +2157,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>26</v>
@@ -2167,7 +2178,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>27</v>

</xml_diff>